<commit_message>
modified:   core/core_chain.py 	new file:   core/output_format_conversion.py 	modified:   core/output_parser.py 	new file:   core/prompt.py 	modified:   core/qa_chain_qianfan.py 	modified:   test.py 	modified:   test.xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>问询事项</t>
+          <t>问询函主题</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -486,22 +486,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>核查并详细说明相关问题</t>
+          <t>关于江苏哈工智能机器人股份有限公司拟变更2023年度会计师事务所的公告</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>你公司于 2024年3月22日晚间披露 《 股票交易 异常波动公告》，称公司对有关事项进行了核查，公司不存在应披露而未披露的重大事项，也不存在处于筹划阶段的重大事项， 3月24日晚间你公司就此予以更正。</t>
+          <t>原聘2023年年审会计师事务所天衡会计师事务所（特殊普通合伙）因人力资源配置和工作安排情况预计无法为江苏哈工智能机器人股份有限公司提供2023年度财务报告的审计服务，江苏哈工智能机器人股份有限公司拟改聘亚太（集团）会计师事务所（特殊普通合伙）为2023年度审计机构，并提交2024年3月21日召开的股东大会审议。股东大会召开日距离江苏哈工智能机器人股份有限公司2023年年报预约披露日（即2024年4月25日）仅约一个月时间。天衡会计师事务所对江苏哈工智能机器人股份有限公司2022年度财务报告出具保留意见、内部控制出具否定意见，江苏哈工智能机器人股份有限公司股票交易因此被实施其他风险警示。截至目前，江苏哈工智能机器人股份有限公司尚存较多对外投资、逾期债务、业绩对赌、重大诉讼等未决事项。</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['自查并说明信息披露差错的原因', '自查并说明重要时间节点、具体参与人员、筹划事项内容等', '自查内幕信息知 情人登记及内幕信息管理情况', '核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况']</t>
+          <t>['自聘任天衡所为2023年度审计机构以来，江苏哈工智能机器人股份有限公司与天衡所就年审事项沟通的具体情况，包括但不限于沟通时间、参与沟通人员、沟通的主要内容等，说明天衡所是否已开展部分审计工作（包括预审），并结合上述情况说明天衡所是否存在审计受限等情况，江苏哈工智能机器人股份有限公司与天衡所在审计工作安排、审计收费、审计调整、审计意见等方面是否存在重大分歧，本次改聘是否存在其他原因。', '说明与亚太所沟通由其承接江苏哈工智能机器人股份有限公司2023年年审工作的筹划过程，直至年报预约披露日前约一个月才改聘年审机构的原因及合理性。', '结合亚太所本次审计工作计划、专业人员配备、目前实际进展等情况，说明亚太所是否充分了解江苏哈工智能机器人股份有限公司面临的生产经营及财务风险、是否有充足时间了解被审计单位及其环境与内部控制、是否有充足时间审慎设计与执行审计程序、是否已做好与前任会计师的沟通工作。', '说明江苏哈工智能机器人股份有限公司存在的较多重大未决事项是否会对新聘年审会计师事务所的工作带来重大困难或障碍，是否不利于年度审计工作的延续性，如是，说明亚太所的应对措施。', '江苏哈工智能机器人股份有限公司审计委员会说明就改聘事项进行的核实、评估过程，并提供工作记录（如有），在此基础上说明审计委员会成员是否已勤勉尽责。', '结合对前述问题的答复，说明江苏哈工智能机器人股份有限公司是否存在购买审计意见、规避其他风险警示的情形，并充分提示相关风险。']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>核查并详细说明相关问题</t>
+          <t>关于江苏哈工智能机器人股份有限公司拟变更2023年度会计师事务所的公告</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>江苏哈工智能机器人股份有限公司</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>2024年3月6日</t>
         </is>
       </c>
     </row>
@@ -536,47 +536,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>详细说明本次重大资产重组事项的筹划过程</t>
+          <t>关于标的资产业务和财务情况</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>本次重组提示性公告披露前， 你公司股价涨幅较大并达到异常波动标准。</t>
+          <t>预案披露，标的公司江苏朗迅工业智能装备有限公司（以下简称江苏朗迅）主营自动化设备的研发、生产和销售，产品应用于消费电子、汽车、医疗等领域。相关公告显示，江苏朗迅向苹果产业链厂商主要销售iPad、笔记本电脑的组装类设备，2023年以来，由于上游客户采购变化，江苏朗迅向苹果产业链厂商直接销售组装类设备，未来相关业务开展存在一定的不确定性。2022年、2023年，江苏朗迅分别实现营业收入 4957.75 万元、9837.75 万元，实现净利润 1422.78 万元、1323.97 万元，其中苹果产业链收入占总收入比例约为 90%、40%。2023 年年末，江苏朗迅资产总额 1.46 亿元，较 2022 年年末同比增加 168%。</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['详细说明本次重大资产重组事项的筹划过程，包括不限于重要时间节点、具体参与人员、筹划事项内容等', '报送内幕知情人名单', '自查内幕信息知 情人登记及内幕信息管理情况', '核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况']</t>
+          <t>['具体说明江苏朗迅的业务模式、所处产业链环节、提供的主要附加值、技术门槛，并结合同行业竞争对手情况说明其市场地位，近两年业绩表现是否符合行业发展趋势；', '分产品列示近两年江苏朗迅主要收入及成本构成、毛利率、净利润及同比变动情况；', '结合江苏朗迅经营模式、在手订单、客户构成、行业地位等，说明江苏朗迅2023年营业收入大幅增长的主要原因；', '说明江苏朗迅苹果产业链收入占比下滑的主要原因，并结合主要客户变动情况和订单获取方式，说明江苏朗迅与相关客户的合作是否具有稳定性与可持续性，并充分提示风险；', '结合产品结构、毛利率变化、同行业可比公司情况，说明江苏朗迅2023年在营业收入大幅增长的情况下净利润下滑的主要原因及合理性；', '说明 2023 年年末江苏朗迅资产总额大幅增加的主要原因，说明本次交易完成后，标的资产的持续运营是否需要大额资金投入，是否有利于提升上市公司财务状况。']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>详细说明本次重大资产重组事项的筹划过程</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -586,47 +586,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>详细说明本次交易构成重大资产重组的测算过程</t>
+          <t>关于标的资产业务和财务情况</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业。</t>
+          <t>预案及相关公告披露，标的公司苏州郎克斯精密五金有限公司（以下简称苏州郎克斯）主营精密金属结构件的研发、生产和销售，主要为苹果产业链厂商提供手机边框等结构件受托加工服务。2022 年、2023 年，苏州郎克斯分别实现营业收入 2.34 亿元、2.35 亿元，实现净利润 2519.71 万元、5786.28 万元，其中苹果产业链收入占总收入比例分别为 96%、89%。</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['结合自身以及标的公司财务数据详细说明本次交易构成重大资产重组的测算过程', '详细说明你公司进入新业务领域的原因，在标的业务与你公司现有主营业务存在较大差异的情况下，如何实现协同效应', '结合你公司进入新领域的专业人员配备、资质情况及业务发展资金储备、资金来源等因素，充分论证进入新业务领域的可行性，收购完成后能否对标的资产实施有效控制', '详细说明新领域的行业竞争情况、平均盈利水平，并说明标的公司的主要业务模式、核心竞争力', '综合前述情况，详细说明本次重组是否符合《重大资产重组管理办法》第十一条有关有利于增强上市公司核心竞争力、有利于上市公司形成或者保持健全有效的法人治理结构等']</t>
+          <t>['补充披露苏州郎克斯所处细分行业的基本情况，包括但不限于市场规模、竞争格局、进入壁垒、技术发展趋势等；', '分产品列示近三年苏州郎克斯与苹果产业链厂商签订的订单金额、交付时间，并分析订单变化原因；', '结合苹果产业链厂商资格的考察认证条件，说明苏州郎克斯维持该供应商资格所依赖的核心资源，分析相关资源的可持续性，说明苏州郎克斯是否存在被替换或订单下降的风险；', '结合上下游行业整体情况、可比公司情况、标的公司产品结构、毛利率变化等，说明苏州郎克斯2023年在营业收入基本持平的情况下净利润大幅增长的主要原因及合理性。']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>详细说明本次交易构成重大资产重组的测算过程</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -636,47 +636,47 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>做好风险提示工作</t>
+          <t>关于交易方案</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>你公司2023年度业绩预告显示， 预计 2023年实现营业收入 3,200.00 万元至3,500.00 万元，实现 归属于母公司净利润为亏损4,000.00万元至4,600.00 万元 ，根据本所《股票上市规则》相关规定，你公司股票将可能于 2023年年报披露后被本所实施退市风险警示处理</t>
+          <t>预案披露，公司拟通过发行股份及支付现金方式，购买江苏朗迅 90%股权、苏州郎克斯 45%股权和苏州晔煜企业管理合伙企业（有限合伙） 23.0769%出资份额，同时募集配套资金。本次交易完成后，公司将在现有皮鞋业务板块上增加精密金属结构件和自动化设备系列产品的研发、生产和销售。</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>严格对照本所相关规则，做好风险提示工作</t>
+          <t>['说明后续在业务、资产、财务、人员、组织机构等方面拟对标的公司实施整合的具体措施及计划安排；', '结合公司现有的经验、人员及技术等储备，以及前述整合措施及计划，说明在主营业务存在较大差异的情况下，公司后续能否对标的公司经营和财务等方面实施有效管控。', '补充披露本次交易各项标的资产的预估值，说明最近一次股权变更的估值作价与本次交易预估值是否存在较大差异，如是，说明原因及合理性。', '补充披露：本次收购苏州郎克斯 45%股权的具体构成，包括交易对方及对应收购比例；本次未收购苏州郎克斯全部股权的原因及主要考虑，是否存在进一步收购剩余股权的计划；结合交易完成后标的资产控制权安排、重大事项决策程序、人员及业务整合计划等，说明公司能否对苏州郎克斯形成有效管控。', '补充披露：上述控股和参股公司的主要股东情况，包括股东名称、出资时间、出资额、与本次交易对方是否存在关联关系等；说明上述控股和参股公司是否专为本次交易设立，相关方是否存在潜在安排；结合交易完成后上述控股和参股公司的重大事项决策程序、人员及业务整合计划等，说明公司能否对上述公司形成有效管控。', '补充披露：苏州郎克斯是否存在因上述事项被相应主管部门处罚的风险；苏州郎克斯降低劳务派遣用工比例的具体措施及其合法合规性，并说明相关措施对苏州郎克斯生产经营及成本费用的影响；结合报告期内标的公司劳务派遣人数规模、后续被处罚风险、拟采取措施等，披露前述事项对本次交易的影响。']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>做好风险提示工作</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -686,22 +686,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>关于本次交易情况</t>
+          <t>其他</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司拟使用超募资金（含利息收入、理财收益等）9,023.81万元用于收购福昕鲲鹏（北京）信息科技有限公司（以下简称福昕鲲鹏或标的公司）38.27%的股权，本次股权收购完成后，公司将持有标的公司73.24%的股权，取得对标的公司的控制权。</t>
+          <t>预案披露，截至 2023 年 12 月 31 日，标的公司苏州郎克斯正式员工人数约300人，高峰时期用工人数超过1000人，除正式员工外，其余均通过劳务派遣方式用工，劳务派遣用工比例存在超过《劳务派遣暂行规定》规定的 10%上限的情形。</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['结合标的公司的实际经营情况、研发团队、研发成果、技术实力、行业地位、近一年同行业公司的并购估值情况等，说明标的公司股东权益评估价值与公司净资产差异较大的原因、依据及其合理性；', '本次交易约定的三期付款先决条件，并说明公司本次交易支付安排是否符合商业惯例、是否有利于保障公司及中小投资者利益；', '公司实施此次股权收购的必要性、决策过程，未设置业绩补偿安排的原因，以及拟采取何种措施保证投资收益、保障公司及中小投资者利益。']</t>
+          <t>['自查内幕信息知情人登记及内幕信息管理情况，核实公司提交的内幕信息知情人名单是否真实、准确、完整；', '补充披露本次重大资产重组的筹划过程，包括但不限于主要时间节点、参与知情人员、商议及决策内容，说明是否存在内幕信息提前泄露情形。']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>关于本次交易情况</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -711,22 +711,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>科创公函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>二〇二四年三月二十五日</t>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -736,37 +736,37 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>关于标的公司经营情况</t>
+          <t>你公司于 2024年3月22日晚间披露 《 股票交易 异常波动公告》，称公司对有关事项进行了核查，公司不存在应披露而未披露的重大事项，也不存在处于筹划阶段的重大事项， 3月24日晚间你公司就此予以更正。 请你公司 就前述信息披露差错的原因予以自查并说明，包括不限于重大事项的内部信息管理、内部核查机制、信息披露内部审查流程等是否完善，相关流程执行中存在的问题，以及整改情况等。</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>公告显示，标的公司净资产为负，最近一年及一期净利润持续亏损，2023年1-10月净亏损达到7,471.04万元。</t>
+          <t>你公司披露的《 股票交易 异常波动公告》存在信息披露差错，需要进行自查并说明。</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['标的公司的资产负债结构、主要资产构成，标的公司的资产是否足以支持业务运营；', '标的公司财产抵押及贷款的现状，说明标的公司是否存在债务清偿风险；', '标的公司最近三年的主要财务数据及业务发展情况，并说明标的公司最近一年及一期连续亏损的原因以及本次收购是否有利于提高上市公司盈利能力。']</t>
+          <t>['自查并说明信息披露差错的原因', '重大事项的内部信息管理情况', '内部核查机制情况', '信息披露内部审查流程情况', '相关流程执行中存在的问题', '整改情况']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>关于标的公司经营情况</t>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>上海证券交易所</t>
+          <t>深圳证券交易所</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>科创公函</t>
+          <t>关注函</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司</t>
+          <t>四川金时科技股份有限公司</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>二〇二四年三月二十五日</t>
+          <t>2024年3月26日</t>
         </is>
       </c>
     </row>
@@ -786,47 +786,1047 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>本次重组提示性公告披露前， 你公司股价涨幅较大并达到异常波动标准。 请详细说明你公司就本次重大资产重组事项的筹划过程，包括不限于重要时间节点、具体参与人员、筹划事项内容等，并报送内幕知情人名单。请自查内幕信息知 情人登记及内幕信息管理情况，并核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况，说明是否存在内幕信息提前泄露的情形。</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>本次重组提示性公告披露前，你公司股价涨幅较大并达到异常波动标准，可能存在内幕信息提前泄露的情形。</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['详细说明你公司就本次重大资产重组事项的筹划过程', '报送内幕知情人名单', '自查内幕信息知 情人登记及内幕信息管理情况', '核实内幕信息知情人近期股票交易情况']</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>公告显示， 本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业。请你公司：（1）结合自身以及标的公司财务数据详细说明本次交易构成重大资产重组的测算过程；（2）详细说明你公司进入新业务领域的原因，在标的业务与你公司现有主营业务存在较大差异的情况下，如何实现协同效应；（3）结合你公司进入新领域的专业人员配备、资质情况及业务发展资金储备、资金来源等因素，充分论证进入新业务领域的可行性，收购完成后能否对标的资产实施有效控制；（4）详细说明新领域的行业竞争情况、平均盈利水平，并说明标的公司的主要业务模式、核心竞争力；（5）综合前述情况，详细说明本次重组是否符合《重大资产重组管理办法》第十一条有关有利于增强上市公司核心竞争力、有利于上市公司形成或者保持健全有效的法人治理结构等。</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业，需要详细说明你公司进入新业务领域的原因、可行性以及本次重组是否符合《重大资产重组管理办法》的相关规定。</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['详细说明本次交易构成重大资产重组的测算过程', '详细说明你公司进入新业务领域的原因', '论证进入新业务领域的可行性', '详细说明新领域的行业竞争情况、平均盈利水平', '说明标的公司的主要业务模式、核心竞争力', '详细说明本次重组是否符合《重大资产重组管理办法》的相关规定']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>你公司2023年度业绩预告显示， 预计 2023年实现营业收入 3,200.00 万元至3,500.00 万元，实现 归属于母公司净利润为亏损4,000.00万元至4,600.00 万元 ，根据本所《股票上市规则》相关规定，你公司股票将可能于 2023年年报披露后被本所实施退市风险警示处理，请严格对照本所相关规则，做好风险提示工作。</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>你公司2023年度业绩预告显示，预计亏损较大，根据相关规定，你公司股票将可能面临退市风险警示处理。</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['严格对照本所相关规则，做好风险提示工作']</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>关于交易方案</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>预案显示，公司拟向贾磊等14名交易对方发行股份并支付现金收购北京领为军融科技有限公司（以下简称标的公司）100%股权。交易对方中，贾磊存在一致行动人邢台领诺、邢台雅惠，合计持有标的公司 41.41%的股权,其他交易对方中包含邢台领擎、科实华盈、力高贰号等多家合伙企业。</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['（1）除预案披露的一致行动关系外，贾磊与邢台领擎等其他交易对方是否存在关联关系、一致行动关系和其他潜在利益安排；（2）结合预案中 2022 年标的公司初步预计需要确认股份支付费用约 1,200 万元的情况，说明标的公司股份支付费用产生的具体原因，包括但不限于对象、时间、股份支付方式、估值、支付作价、公允价格及确定依据和其他相关安排，并说明本次交易的预计估值区间与前期股份支付对应估值是否存在差异及原因；（3）结合问题（1）和问题（2） ，说明本次向交易对方发行股份是否可能影响上市公司控制权稳定性，本次交易是否将导致上市公司主营业务发生根本变化，是否可能构成《重大资产重组管理办法》规定的重组上市情形。']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>关于交易对方</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>预案显示：本次发行股份的交易对方为标的公司的 14名股东，其中包括 7家合伙企业。</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['（1）交易对方穿透后的合计人数，说明是否超过 200 人，是否符合《非上市公众公司监管指引第 4 号》相关规定；（2）交易对方是否专为本次交易设立，如是，补充披露交易完成后最终出资的法人或自然人持有合伙企业份额的锁定安排。']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>关于标的核心竞争力</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>预案显示，标的公司主营业务为军事航空仿真系列产品的研制、生产及相关技术服务，核心产品为“通用数字空战仿真系统”，受专业方向和相关资质许可限制，民营军事仿真市场的准入门槛较高，标的公司形成了多项拥有自主知识产权的现金技术，人才及团队优势也是标的公司核心竞争力之一。</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['（1）结合标的公司所在行业市场规模、竞争格局、发展趋势、产业政策、资质许可要求、同行业主要竞争对手情况等，进一步说明标的公司的核心竞争力；（2）结合标的公司产品自主知识产权的取得情况，说明标的公司核心产品是否具备足够的技术先进性及技术壁垒，并充分提示技术迭代风险；（3）结合标的公司核心技术人员的学历构成、相关履历、在标的公司的工作年限等，进一步说明标的公司的人才稳定性情况及竞争优势。']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>关于标的财务状况</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>预案显示，近两年一期标的公司经营业绩波动较大，2022 年营业收入和净利润同比分别增长 81.97%、83.17%，但 2023 年 1-10 月，标的公司实现的营业收入和净利润分别仅达到 2022 年全年的 61.92%和 47.44%。2021 年末，标的公司所有者权益合计为-4,061.85万元。</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['（1）标的公司报告期内经营业绩波动较大的具体原因，相关业绩表现是否与同业公司存在较大差异及其合理性；（2）结合标的公司获取订单的主要方式、在手订单及执行情况、收入确认政策等，是否存在业绩持续下滑风险；（3）标的公司近两年一期前五大客户的销售额及占比、销售模式、是否为关联方，结合主要客户变动情况和客户集中度，说明标的公司是否存在对重大客户依赖的情形及关键客户流失风险；（4）标的公司近两年一期的资产负债的具体构成、资产负债大幅变化的具体原因，收购完成后标的公司相关债务的偿付安排，并结合公司目前的资金状况，说明其是否可能对公司流动性造成不利影响和具体应对措施。']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>关于跨界收购</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>预案显示，公司主营电梯门系统等电梯零部件业务。前期公告显示，公司曾于2020年披露跨界重组预案，拟收购主营换电型新能源汽车零部件等业务的伯坦科技， 2021 年 1 月公告终止重组。本次公司拟再次跨界收购，标的公司主营军事航空仿真系列产品等业务，与公司主营业务不具有协同效应。</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['（1）多次筹划收购与公司主营业务不具有协同效应标的公司的具体原因，充分论证收购的必要性，交易是否符合《重大资产重组管理办法》第十一条的有关规定；（2）结合公司现阶段主营业务、人才储备等情况是否具备足够的整合管控标的公司的能力，审慎推进本次收购事项，并严格按照规则要求履行信息披露义务。']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>关于内幕信息</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>因筹划重大资产重组，公司于 2023 年11 月 6 日起停牌。公司提交停牌申请当日，停牌前筹划本次重大资产重组事项的具体协商、参与知情人自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['（1）停牌前筹划本次重大资产重组事项的具体协商、参与知情人；（2）自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>展鹏科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>关于交易标的的并表</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>预案显示，交易完成后，上市公司、上海宝信软件股份有限公司（以下简称“宝信软件”）分别持有上海地铁电子科技有限公司（以下简称“地铁电科”）50%股权，股权比例相同；上市公司、上海地铁维护保障有限公司（以下简称 “维保公司 ”）将分别持有上海地铁物业管理有限公司（以下简称 “地铁物业 ”）51%、49%股权，股权比例相近。</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['结合地铁电科、地铁物业的公司章程规定、董事会席位安排、经营决策具体安排及重大事项表决安排等，说明交易后上市公司能否对交易标的实施控制、能否将其纳入合并报表及相应会计处理的合理性。']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>关于独立性</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>预案显示，地铁电科主营轨道交通车辆及相关系统部件的维护、维修，地铁物业主营列车等保洁、车站服务设施综合管理。</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['补充披露： （1）地铁电科、地铁物业报告期内是否存在关联销售，若存在，请披露报告期内金额、占比、定价模式及定价公允性；（2）本次交易前后关联交易的金额及规模占比变化情况，本次交易是否有利于减少关联交易、增强上市公司独立性；（3）上市公司后续保持关联交易定价公允、减少和规范关联交易的具体措施。']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>关于地铁电科资产负债率</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>地铁电科报告期内资产负债率分别为74%、70%和69%，远高于上市公司2023年三季度末资产负债率39.53%。</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['补充披露： （1）报告期内地铁电科的资产、负债主要构成，结合自身经营情况、融资来源及融资结构等，说明地铁电科资产负债率较高的原因及合理性；（2）说明此次交易是否会对上市公司财务结构产生重大影响，交易完成后上市公司资产负债率是否处于合理水平。']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>关于地铁电科业绩</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>预案显示，地铁电科报告期内实现营业收入分别为17,696.24万元、13,632.78万元及9,728.3万元，净利润分别为 2,357.88 万元、1,389.45 万元、604.54 万元，净利率分别为13%、10%、6%，净利率持续下降；经营活动产生的现金流量净额分别为-515.36万元、-1,522.17万元及774万元，波动较大。</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['补充披露： （1）结合地铁电科业务开展情况，包括主要客户变化、销售模式、收入确认方式等，说明公司营业收入、净利率下降的原因及合理性；（2）结合公司对客户及供应商的结算方式，说明经营活动现金流量净额波动较大的原因及合理性。']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>关于地铁物业业绩</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>预案显示，地铁物业处于劳动密集型行业，2022 年实现营业收入 21,096.63 万元，同比增长 21%；净利润为 401.34 万元，同比下降 53%，经营活动现金净额为-2,074.36 万元，2021 年同期为-382.58 万元，净利润、经营活动现金净额的变动趋势与营业收入相反，且 2022 年净利率仅为 2%。</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['补充披露： （1）地铁物业的盈利模式，净利率较低的原因及合理性，是否与同行业可比公司相一致；（2）结合前述问题分析、地铁物业经营情况、收入确认方式与期间费用变化等，说明2022年收入大幅提升，但净利润大幅下滑的原因及合理性；（3）结合主要客户及供应商变化情况、结算政策等，说明经营活动现金净额与收入变化不匹配的原因及合理性。']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>关于地铁电科核心竞争力</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>预案显示，地铁电科属于技术密集型行业，核心管理人员及技术人员对其发展至关重要。</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['结合地铁电科所处细分行业竞争格局、同行业竞争对手情况、现有技术储备、人员配置等，说明地铁电科核心竞争力，及此次交易完成后，公司拟采取何种措施整合地铁电科的技术和相关人员。']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>上海申通地铁股份有限公司</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3403</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>关于本次交易情况</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>你公司披露《关于使用超募资金对外投资的公告》称，公司拟使用超募资金（含利息收入、理财收益等）9,023.81万元用于收购福昕鲲鹏（北京）信息科技有限公司（以下简称福昕鲲鹏或标的公司）38.27%的股权，本次股权收购完成后，你公司将持有标的公司73.24%的股权，取得对标的公司的控制权。</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['结合标的公司的实际经营情况、研发团队、研发成果、技术实力、行业地位、近一年同行业公司的并购估值情况等，说明标的公司股东权益评估价值与公司净资产差异较大的原因、依据及其合理性；', '本次交易约定的三期付款先决条件，并说明公司本次交易支付安排是否符合商业惯例、是否有利于保障公司及中小投资者利益；', '公司实施此次股权收购的必要性、决策过程，未设置业绩补偿安排的原因，以及拟采取何种措施保证投资收益、保障公司及中小投资者利益。']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>上证科创公函</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>福建福昕软件开发股份有限公司</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0034</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>关于标的公司经营情况</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>公告显示，标的公司净资产为负，最近一年及一期净利润持续亏损，2023年1-10月净亏损达到7,471.04万元。</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['标的公司的资产负债结构、主要资产构成，标的公司的资产是否足以支持业务运营；', '标的公司财产抵押及贷款的现状，说明标的公司是否存在债务清偿风险；', '标的公司最近三年的主要财务数据及业务发展情况，并说明标的公司最近一年及一期连续亏损的原因以及本次收购是否有利于提高上市公司盈利能力。']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>上证科创公函</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>福建福昕软件开发股份有限公司</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>0034</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>关于后续整合安排</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>公告显示，本次交易完成后，公司将持有标的公司73.24%的股权，取得对标的公司的控制权，标的公司将纳入公司合并报表范围。</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>['本次交易后的董事会及管理层的人员安排，以及公司在业务、资产、财务、人员等方面拟采取的其他整合管控措施，并说明相关安排或措施如何保障对标的公司实现有效整合；', '收购后对标的公司有无进一步资金投入规划，有无收购相关业务领域其他资产的计划，如有，请披露预计投入金额及具体内容；', '结合标的公司产品的具体种类、主要客户及在手订单，细分市场总体规模及行业竞争状况等因素预计标的公司未来三年的收入流情况，是否能够实现业绩扭亏为盈，并说明改善标的公司经营情况的具体举措。']</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>关于后续整合安排</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>上海证券交易所</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['本次交易后的董事会及管理层的人员安排，以及你公司在业务、资产、财务、人员等方面拟采取的其他整合管控措施，并说明相关安排或措施如何保障对标的公司实现有效整合；', '收购后对标的公司有无进一步资金投入规划，有无收购相关业务领域其他资产的计划，如有，请披露预计投入金额及具体内容；', '结合标的公司产品的具体种类、主要客户及在手订单，细分市场总体规模及行业竞争状况等因素预计标的公司未来三年的收入流情况，是否能够实现业绩扭亏为盈，并说明改善标的公司经营情况的具体举措。']</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>上证科创公函</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>福建福昕软件开发股份有限公司</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>0034</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>公司2023年度业绩情况</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>公司2023年财务数据对公司具有较大影响，根据本所《股票上市规则》第 13.1.1条等有关规定，现请你公司进一步核实并补充披露以下事项。</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['区分产品类别披露主营业务的开展情况，包括开展期限、采购及销售模式、收入确认方式等，说明是否为贸易业务', '各业务板块的主要供应商和客户名称、所涉关联关系、业务内容及报告期内变化情况，结合主要合同条款及公司承担的责任和义务等情况，说明报告期内业务收入确认的依据及政策，是否符合《企业会计准则》的规定，是否存在提前确认收入的情形', '结合经营情况、财务状况及变化趋势，说明持续经营能力是否存在重大不确定性，并充分提示风险']</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>关于精伦电子股份有限公司业绩预告相关事项的问询函</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>问询函</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>精伦电子股份有限公司</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十六日</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>营业收入扣除项目及其具体情况</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>请公司补充披露营业收入扣除项目及其具体情况 ，并逐条对照《上海证券交易所上市公司自律监管指南第 2号—业务办理》附件第七号《财务类退市指标：营业收入扣除》有关规定，说明公司未扣除收入的相关业务是否存在应扣除收入未按规定扣除的情况。如扣除后的营业收入等财务指标触及财务类退市情形的，公司股票将被实施退市风险警示 ，请公司充分提示相关风险。</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['营业收入扣除项目及其具体情况']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>关于精伦电子股份有限公司业绩预告相关事项的问询函</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>问询函</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>精伦电子股份有限公司</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十六日</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>关于江苏迈信林航空科技股份有限公司签订战略框架协议暨开展新业务相关事项的问询</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>江苏迈信林航空科技股份有限公司披露《关于自愿披露签订战略框架协议暨开展新业务的公告》称，公司通过子公司苏州瑞盈智算科技有限公司开展算力服务业务，并与苏州算力科技有限公司签订战略合作框架协议，拟在算力领域开展深度合作，建立长期的战略合作关系。经事后审核，根据《上海证券交易所科创板股票上市规则》第14.1.1条，请你公司就如下信息予以说明并补充披露。</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['瑞盈智算的股权结构，预计注册资本实缴到位时间', '结合从事算力服务业务所需要的技术、资质、人员条件及市场竞争情况等，说明公司是否具备相关储备，是否具备开展算力服务业务的条件，是否具备竞争优势，并针对性提示风险', '后续服务器采购计划和具体安排，交付是否存在不确定性', '结合公司的自有资金情况，说明相关投资是否影响公司现金流，是否可能导致公司后续存在资金周转风险', '瑞盈智算后续获取银行信贷，是否需要公司提供担保或承担连带责任，结合后续算力服务业务的不确定性，评估可能给公司带来风险并进行针对性风险提示', '截至目前，上市公司已采购60余台服务器，待瑞盈智算正式运营，公司将以公允价格全部划转至瑞盈智算。请公司补充披露相关采购事项是否达到信息披露标准，智算受让公司已采购服务器的具体安排，包括但不限于转让时间、数量、价格等', '苏州算力科技协助瑞盈智算运营管理的具体工作内容及收费模式，苏州算力科技是否具备资金、技术、客户资源等合作条件']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>关于江苏迈信林航空科技股份有限公司签订战略框架协议暨开展新业务相关事项的问询</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>科创公函</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>福建福昕软件开发股份有限公司</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>未知</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>二〇二四年三月二十五日</t>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>江苏迈信林航空科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0033</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>2024年3月23日</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   core/core_chain.py 	modified:   core/output_parser.py 	modified:   core/prompt.py 	modified:   core/qa_chain_qianfan.py 	deleted:    core/test_pdf.py 	modified:   test.py 	modified:   test.xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,56 @@
           <t>公告日期</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>监管问题</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>监管问题背景</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>需要问询公司的具体方面</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>监管问题类别</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>问询函主题</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>问询机构</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>函件类别</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>公司名称</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>证券代码</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>公告日期</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -491,12 +541,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>原聘2023年年审会计师事务所天衡会计师事务所（特殊普通合伙）因人力资源配置和工作安排情况预计无法为江苏哈工智能机器人股份有限公司提供2023年度财务报告的审计服务，江苏哈工智能机器人股份有限公司拟改聘亚太（集团）会计师事务所（特殊普通合伙）为2023年度审计机构，并提交2024年3月21日召开的股东大会审议。股东大会召开日距离江苏哈工智能机器人股份有限公司2023年年报预约披露日（即2024年4月25日）仅约一个月时间。天衡会计师事务所对江苏哈工智能机器人股份有限公司2022年度财务报告出具保留意见、内部控制出具否定意见，江苏哈工智能机器人股份有限公司股票交易因此被实施其他风险警示。截至目前，江苏哈工智能机器人股份有限公司尚存较多对外投资、逾期债务、业绩对赌、重大诉讼等未决事项。</t>
+          <t>原聘2023年年审会计师事务所天衡会计师事务所（特殊普通合伙）因人力资源配置和工作安排情况预计无法为江苏哈工智能机器人股份有限公司提供2023年度财务报告的审计服务，江苏哈工智能机器人股份有限公司拟改聘亚太（集团）会计师事务所（特殊普通合伙）为2023年度审计机构，并提交2024年3月21日召开的股东大会审议。股东大会召开日距离江苏哈工智能机器人股份有限公司2023年年报预约披露日（即2024年4月25日）仅约一个月时间。天衡所对江苏哈工智能机器人股份有限公司2022年度财务报告出具保留意见、内部控制出具否定意见，江苏哈工智能机器人股份有限公司股票交易因此被实施其他风险警示。截至目前，江苏哈工智能机器人股份有限公司尚存较多对外投资、逾期债务、业绩对赌、重大诉讼等未决事项。</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['自聘任天衡所为2023年度审计机构以来，江苏哈工智能机器人股份有限公司与天衡所就年审事项沟通的具体情况，包括但不限于沟通时间、参与沟通人员、沟通的主要内容等，说明天衡所是否已开展部分审计工作（包括预审），并结合上述情况说明天衡所是否存在审计受限等情况，江苏哈工智能机器人股份有限公司与天衡所在审计工作安排、审计收费、审计调整、审计意见等方面是否存在重大分歧，本次改聘是否存在其他原因。', '说明与亚太所沟通由其承接江苏哈工智能机器人股份有限公司2023年年审工作的筹划过程，直至年报预约披露日前约一个月才改聘年审机构的原因及合理性。', '结合亚太所本次审计工作计划、专业人员配备、目前实际进展等情况，说明亚太所是否充分了解江苏哈工智能机器人股份有限公司面临的生产经营及财务风险、是否有充足时间了解被审计单位及其环境与内部控制、是否有充足时间审慎设计与执行审计程序、是否已做好与前任会计师的沟通工作。', '说明江苏哈工智能机器人股份有限公司存在的较多重大未决事项是否会对新聘年审会计师事务所的工作带来重大困难或障碍，是否不利于年度审计工作的延续性，如是，说明亚太所的应对措施。', '江苏哈工智能机器人股份有限公司审计委员会说明就改聘事项进行的核实、评估过程，并提供工作记录（如有），在此基础上说明审计委员会成员是否已勤勉尽责。', '结合对前述问题的答复，说明江苏哈工智能机器人股份有限公司是否存在购买审计意见、规避其他风险警示的情形，并充分提示相关风险。']</t>
+          <t>['列示自聘任天衡所为2023年度审计机构以来，江苏哈工智能机器人股份有限公司与天衡所就年审事项沟通的具体情况，包括但不限于沟通时间、参与沟通人员、沟通的主要内容等，说明天衡所是否已开展部分审计工作（包括预审），并结合上述情况说明天衡所是否存在审计受限等情况，江苏哈工智能机器人股份有限公司与天衡所在审计工作安排、审计收费、审计调整、审计意见等方面是否存在重大分歧，本次改聘是否存在其他原因。', '说明与亚太所沟通由其承接江苏哈工智能机器人股份有限公司2023年年审工作的筹划过程，直至年报预约披露日前约一个月才改聘年审机构的原因及合理性。', '结合亚太所本次审计工作计划、专业人员配备、目前实际进展等情况，说明亚太所是否充分了解江苏哈工智能机器人股份有限公司面临的生产经营及财务风险、是否有充足时间了解被审计单位及其环境与内部控制、是否有充足时间审慎设计与执行审计程序、是否已做好与前任会计师的沟通工作。', '说明江苏哈工智能机器人股份有限公司存在的较多重大未决事项是否会对新聘年审会计师事务所的工作带来重大困难或障碍，是否不利于年度审计工作的延续性，如是，说明亚太所的应对措施。', '请江苏哈工智能机器人股份有限公司审计委员会说明就改聘事项进行的核实、评估过程，并提供工作记录（如有），在此基础上说明审计委员会成员是否已勤勉尽责。', '结合对前述问题的答复，说明江苏哈工智能机器人股份有限公司是否存在购买审计意见、规避其他风险警示的情形，并充分提示相关风险。', '请江苏哈工智能机器人股份有限公司将深圳证券交易所曾于2024年1月19日向天衡所发出的《关于对江苏哈工智能机器人股份有限公司2023年财务会计报告审计相关事项的提示函》转达亚太所，并提供送达回执。']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -525,6 +575,56 @@
         </is>
       </c>
       <c r="J2" t="inlineStr">
+        <is>
+          <t>2024年3月6日</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>关于江苏哈工智能机器人股份有限公司拟变更2023年度会计师事务所的公告</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>原聘2023年年审会计师事务所天衡会计师事务所（特殊普通合伙）因人力资源配置和工作安排情况预计无法为江苏哈工智能机器人股份有限公司提供2023年度财务报告的审计服务，江苏哈工智能机器人股份有限公司拟改聘亚太（集团）会计师事务所（特殊普通合伙）为2023年度审计机构，并提交2024年3月21日召开的股东大会审议。股东大会召开日距离江苏哈工智能机器人股份有限公司2023年年报预约披露日（即2024年4月25日）仅约一个月时间。天衡所对江苏哈工智能机器人股份有限公司2022年度财务报告出具保留意见、内部控制出具否定意见，江苏哈工智能机器人股份有限公司股票交易因此被实施其他风险警示。截至目前，江苏哈工智能机器人股份有限公司尚存较多对外投资、逾期债务、业绩对赌、重大诉讼等未决事项。</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>['列示自聘任天衡所为2023年度审计机构以来，江苏哈工智能机器人股份有限公司与天衡所就年审事项沟通的具体情况，包括但不限于沟通时间、参与沟通人员、沟通的主要内容等，说明天衡所是否已开展部分审计工作（包括预审），并结合上述情况说明天衡所是否存在审计受限等情况，江苏哈工智能机器人股份有限公司与天衡所在审计工作安排、审计收费、审计调整、审计意见等方面是否存在重大分歧，本次改聘是否存在其他原因。', '说明与亚太所沟通由其承接江苏哈工智能机器人股份有限公司2023年年审工作的筹划过程，直至年报预约披露日前约一个月才改聘年审机构的原因及合理性。', '结合亚太所本次审计工作计划、专业人员配备、目前实际进展等情况，说明亚太所是否充分了解江苏哈工智能机器人股份有限公司面临的生产经营及财务风险、是否有充足时间了解被审计单位及其环境与内部控制、是否有充足时间审慎设计与执行审计程序、是否已做好与前任会计师的沟通工作。', '说明江苏哈工智能机器人股份有限公司存在的较多重大未决事项是否会对新聘年审会计师事务所的工作带来重大困难或障碍，是否不利于年度审计工作的延续性，如是，说明亚太所的应对措施。', '请江苏哈工智能机器人股份有限公司审计委员会说明就改聘事项进行的核实、评估过程，并提供工作记录（如有），在此基础上说明审计委员会成员是否已勤勉尽责。', '结合对前述问题的答复，说明江苏哈工智能机器人股份有限公司是否存在购买审计意见、规避其他风险警示的情形，并充分提示相关风险。', '请江苏哈工智能机器人股份有限公司将深圳证券交易所曾于2024年1月19日向天衡所发出的《关于对江苏哈工智能机器人股份有限公司2023年财务会计报告审计相关事项的提示函》转达亚太所，并提供送达回执。']</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>定期报告披露问题</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>关于江苏哈工智能机器人股份有限公司拟变更2023年度会计师事务所的公告</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>江苏哈工智能机器人股份有限公司</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
         <is>
           <t>2024年3月6日</t>
         </is>
@@ -546,7 +646,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>['具体说明江苏朗迅的业务模式、所处产业链环节、提供的主要附加值、技术门槛，并结合同行业竞争对手情况说明其市场地位，近两年业绩表现是否符合行业发展趋势；', '分产品列示近两年江苏朗迅主要收入及成本构成、毛利率、净利润及同比变动情况；', '结合江苏朗迅经营模式、在手订单、客户构成、行业地位等，说明江苏朗迅2023年营业收入大幅增长的主要原因；', '说明江苏朗迅苹果产业链收入占比下滑的主要原因，并结合主要客户变动情况和订单获取方式，说明江苏朗迅与相关客户的合作是否具有稳定性与可持续性，并充分提示风险；', '结合产品结构、毛利率变化、同行业可比公司情况，说明江苏朗迅2023年在营业收入大幅增长的情况下净利润下滑的主要原因及合理性；', '说明 2023 年年末江苏朗迅资产总额大幅增加的主要原因，说明本次交易完成后，标的资产的持续运营是否需要大额资金投入，是否有利于提升上市公司财务状况。']</t>
+          <t>['具体说明江苏朗迅的业务模式、所处产业链环节、提供的主要附加值、技术门槛，并结合同行业竞争对手情况说明其市场地位，近两年业绩表现是否符合行业发展趋势', '分产品列示近两年江苏朗迅主要收入及成本构成、毛利率、净利润及同比变动情况', '结合江苏朗迅经营模式、在手订单、客户构成、行业地位等，说明江苏朗迅2023年营业收入大幅增长的主要原因', '说明江苏朗迅苹果产业链收入占比下滑的主要原因，并结合主要客户变动情况和订单获取方式，说明江苏朗迅与相关客户的合作是否具有稳定性与可持续性，并充分提示风险', '结合产品结构、毛利率变化、同行业可比公司情况，说明江苏朗迅2023年在营业收入大幅增长的情况下净利润下滑的主要原因及合理性', '说明 2023 年年末江苏朗迅资产总额大幅增加的主要原因，说明本次交易完成后，标的资产的持续运营是否需要大额资金投入，是否有利于提升上市公司财务状况']</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -575,6 +675,56 @@
         </is>
       </c>
       <c r="J3" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>关于标的资产业务和财务情况</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>预案披露，标的公司江苏朗迅工业智能装备有限公司（以下简称江苏朗迅）主营自动化设备的研发、生产和销售，产品应用于消费电子、汽车、医疗等领域。相关公告显示，江苏朗迅向苹果产业链厂商主要销售iPad、笔记本电脑的组装类设备，2023年以来，由于上游客户采购变化，江苏朗迅向苹果产业链厂商直接销售组装类设备，未来相关业务开展存在一定的不确定性。2022年、2023年，江苏朗迅分别实现营业收入 4957.75 万元、9837.75 万元，实现净利润 1422.78 万元、1323.97 万元，其中苹果产业链收入占总收入比例约为 90%、40%。2023 年年末，江苏朗迅资产总额 1.46 亿元，较 2022 年年末同比增加 168%。</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>['具体说明江苏朗迅的业务模式、所处产业链环节、提供的主要附加值、技术门槛，并结合同行业竞争对手情况说明其市场地位，近两年业绩表现是否符合行业发展趋势', '分产品列示近两年江苏朗迅主要收入及成本构成、毛利率、净利润及同比变动情况', '结合江苏朗迅经营模式、在手订单、客户构成、行业地位等，说明江苏朗迅2023年营业收入大幅增长的主要原因', '说明江苏朗迅苹果产业链收入占比下滑的主要原因，并结合主要客户变动情况和订单获取方式，说明江苏朗迅与相关客户的合作是否具有稳定性与可持续性，并充分提示风险', '结合产品结构、毛利率变化、同行业可比公司情况，说明江苏朗迅2023年在营业收入大幅增长的情况下净利润下滑的主要原因及合理性', '说明 2023 年年末江苏朗迅资产总额大幅增加的主要原因，说明本次交易完成后，标的资产的持续运营是否需要大额资金投入，是否有利于提升上市公司财务状况']</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>重大资产重组问题</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
         <is>
           <t>二〇二四年一月二十四日</t>
         </is>
@@ -596,7 +746,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>['补充披露苏州郎克斯所处细分行业的基本情况，包括但不限于市场规模、竞争格局、进入壁垒、技术发展趋势等；', '分产品列示近三年苏州郎克斯与苹果产业链厂商签订的订单金额、交付时间，并分析订单变化原因；', '结合苹果产业链厂商资格的考察认证条件，说明苏州郎克斯维持该供应商资格所依赖的核心资源，分析相关资源的可持续性，说明苏州郎克斯是否存在被替换或订单下降的风险；', '结合上下游行业整体情况、可比公司情况、标的公司产品结构、毛利率变化等，说明苏州郎克斯2023年在营业收入基本持平的情况下净利润大幅增长的主要原因及合理性。']</t>
+          <t>['补充披露苏州郎克斯所处细分行业的基本情况，包括但不限于市场规模、竞争格局、进入壁垒、技术发展趋势等', '分产品列示近三年苏州郎克斯与苹果产业链厂商签订的订单金额、交付时间，并分析订单变化原因', '结合苹果产业链厂商资格的考察认证条件，说明苏州郎克斯维持该供应商资格所依赖的核心资源，分析相关资源的可持续性，说明苏州郎克斯是否存在被替换或订单下降的风险', '结合上下游行业整体情况、可比公司情况、标的公司产品结构、毛利率变化等，说明苏州郎克斯2023年在营业收入基本持平的情况下净利润大幅增长的主要原因及合理性']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -625,6 +775,56 @@
         </is>
       </c>
       <c r="J4" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>关于标的资产业务和财务情况</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>预案及相关公告披露，标的公司苏州郎克斯精密五金有限公司（以下简称苏州郎克斯）主营精密金属结构件的研发、生产和销售，主要为苹果产业链厂商提供手机边框等结构件受托加工服务。2022 年、2023 年，苏州郎克斯分别实现营业收入 2.34 亿元、2.35 亿元，实现净利润 2519.71 万元、5786.28 万元，其中苹果产业链收入占总收入比例分别为 96%、89%。</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>['补充披露苏州郎克斯所处细分行业的基本情况，包括但不限于市场规模、竞争格局、进入壁垒、技术发展趋势等', '分产品列示近三年苏州郎克斯与苹果产业链厂商签订的订单金额、交付时间，并分析订单变化原因', '结合苹果产业链厂商资格的考察认证条件，说明苏州郎克斯维持该供应商资格所依赖的核心资源，分析相关资源的可持续性，说明苏州郎克斯是否存在被替换或订单下降的风险', '结合上下游行业整体情况、可比公司情况、标的公司产品结构、毛利率变化等，说明苏州郎克斯2023年在营业收入基本持平的情况下净利润大幅增长的主要原因及合理性']</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>重大资产重组问题</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
         <is>
           <t>二〇二四年一月二十四日</t>
         </is>
@@ -646,7 +846,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>['说明后续在业务、资产、财务、人员、组织机构等方面拟对标的公司实施整合的具体措施及计划安排；', '结合公司现有的经验、人员及技术等储备，以及前述整合措施及计划，说明在主营业务存在较大差异的情况下，公司后续能否对标的公司经营和财务等方面实施有效管控。', '补充披露本次交易各项标的资产的预估值，说明最近一次股权变更的估值作价与本次交易预估值是否存在较大差异，如是，说明原因及合理性。', '补充披露：本次收购苏州郎克斯 45%股权的具体构成，包括交易对方及对应收购比例；本次未收购苏州郎克斯全部股权的原因及主要考虑，是否存在进一步收购剩余股权的计划；结合交易完成后标的资产控制权安排、重大事项决策程序、人员及业务整合计划等，说明公司能否对苏州郎克斯形成有效管控。', '补充披露：上述控股和参股公司的主要股东情况，包括股东名称、出资时间、出资额、与本次交易对方是否存在关联关系等；说明上述控股和参股公司是否专为本次交易设立，相关方是否存在潜在安排；结合交易完成后上述控股和参股公司的重大事项决策程序、人员及业务整合计划等，说明公司能否对上述公司形成有效管控。', '补充披露：苏州郎克斯是否存在因上述事项被相应主管部门处罚的风险；苏州郎克斯降低劳务派遣用工比例的具体措施及其合法合规性，并说明相关措施对苏州郎克斯生产经营及成本费用的影响；结合报告期内标的公司劳务派遣人数规模、后续被处罚风险、拟采取措施等，披露前述事项对本次交易的影响。']</t>
+          <t>['说明后续在业务、资产、财务、人员、组织机构等方面拟对标的公司实施整合的具体措施及计划安排', '结合公司现有的经验、人员及技术等储备，以及前述整合措施及计划，说明在主营业务存在较大差异的情况下，公司后续能否对标的公司经营和财务等方面实施有效管控']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -675,6 +875,56 @@
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>关于交易方案</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>预案披露，公司拟通过发行股份及支付现金方式，购买江苏朗迅 90%股权、苏州郎克斯 45%股权和苏州晔煜企业管理合伙企业（有限合伙） 23.0769%出资份额，同时募集配套资金。本次交易完成后，公司将在现有皮鞋业务板块上增加精密金属结构件和自动化设备系列产品的研发、生产和销售。</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>['说明后续在业务、资产、财务、人员、组织机构等方面拟对标的公司实施整合的具体措施及计划安排', '结合公司现有的经验、人员及技术等储备，以及前述整合措施及计划，说明在主营业务存在较大差异的情况下，公司后续能否对标的公司经营和财务等方面实施有效管控']</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>重大资产重组问题</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
         <is>
           <t>二〇二四年一月二十四日</t>
         </is>
@@ -686,17 +936,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>其他</t>
+          <t>关于交易方案</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>预案披露，截至 2023 年 12 月 31 日，标的公司苏州郎克斯正式员工人数约300人，高峰时期用工人数超过1000人，除正式员工外，其余均通过劳务派遣方式用工，劳务派遣用工比例存在超过《劳务派遣暂行规定》规定的 10%上限的情形。</t>
+          <t>预案披露，2023 年 1 月，公司向江苏朗迅增资 2000 万元，持有江苏朗迅增资后 10%的股权。</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>['自查内幕信息知情人登记及内幕信息管理情况，核实公司提交的内幕信息知情人名单是否真实、准确、完整；', '补充披露本次重大资产重组的筹划过程，包括但不限于主要时间节点、参与知情人员、商议及决策内容，说明是否存在内幕信息提前泄露情形。']</t>
+          <t>['补充披露本次交易各项标的资产的预估值，说明最近一次股权变更的估值作价与本次交易预估值是否存在较大差异，如是，说明原因及合理性']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -725,6 +975,56 @@
         </is>
       </c>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>关于交易方案</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>预案披露，2023 年 1 月，公司向江苏朗迅增资 2000 万元，持有江苏朗迅增资后 10%的股权。</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>['补充披露本次交易各项标的资产的预估值，说明最近一次股权变更的估值作价与本次交易预估值是否存在较大差异，如是，说明原因及合理性']</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>重大资产重组问题</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
         <is>
           <t>二〇二四年一月二十四日</t>
         </is>
@@ -736,47 +1036,97 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>你公司于 2024年3月22日晚间披露 《 股票交易 异常波动公告》，称公司对有关事项进行了核查，公司不存在应披露而未披露的重大事项，也不存在处于筹划阶段的重大事项， 3月24日晚间你公司就此予以更正。 请你公司 就前述信息披露差错的原因予以自查并说明，包括不限于重大事项的内部信息管理、内部核查机制、信息披露内部审查流程等是否完善，相关流程执行中存在的问题，以及整改情况等。</t>
+          <t>关于交易方案</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>你公司披露的《 股票交易 异常波动公告》存在信息披露差错，需要进行自查并说明。</t>
+          <t>预案披露，苏州郎克斯共有 4 名股东，其中周泽臣持有 65%的股权，苏州晔煜持有13%的股权，王永富和黄永强各持有11%的股权，周泽臣为苏州郎克斯的实际控制人。本次交易完成后，公司将直接持有苏州郎克斯 45%的股权，同时通过收购苏州晔煜间接持有苏州郎克斯13%的股权，合计持股比例58%。</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>['自查并说明信息披露差错的原因', '重大事项的内部信息管理情况', '内部核查机制情况', '信息披露内部审查流程情况', '相关流程执行中存在的问题', '整改情况']</t>
+          <t>['本次收购苏州郎克斯 45%股权的具体构成，包括交易对方及对应收购比例', '本次未收购苏州郎克斯全部股权的原因及主要考虑，是否存在进一步收购剩余股权的计划', '结合交易完成后标的资产控制权安排、重大事项决策程序、人员及业务整合计划等，说明公司能否对苏州郎克斯形成有效管控']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>关于对四川金时科技股份有限公司的 关注函</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>关于交易方案</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>预案披露，苏州郎克斯共有 4 名股东，其中周泽臣持有 65%的股权，苏州晔煜持有13%的股权，王永富和黄永强各持有11%的股权，周泽臣为苏州郎克斯的实际控制人。本次交易完成后，公司将直接持有苏州郎克斯 45%的股权，同时通过收购苏州晔煜间接持有苏州郎克斯13%的股权，合计持股比例58%。</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['本次收购苏州郎克斯 45%股权的具体构成，包括交易对方及对应收购比例', '本次未收购苏州郎克斯全部股权的原因及主要考虑，是否存在进一步收购剩余股权的计划', '结合交易完成后标的资产控制权安排、重大事项决策程序、人员及业务整合计划等，说明公司能否对苏州郎克斯形成有效管控']</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>重大资产重组问题</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -786,47 +1136,97 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>本次重组提示性公告披露前， 你公司股价涨幅较大并达到异常波动标准。 请详细说明你公司就本次重大资产重组事项的筹划过程，包括不限于重要时间节点、具体参与人员、筹划事项内容等，并报送内幕知情人名单。请自查内幕信息知 情人登记及内幕信息管理情况，并核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况，说明是否存在内幕信息提前泄露的情形。</t>
+          <t>其他</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>本次重组提示性公告披露前，你公司股价涨幅较大并达到异常波动标准，可能存在内幕信息提前泄露的情形。</t>
+          <t>预案披露，截至 2023 年 12 月 31 日，标的公司苏州郎克斯正式员工人数约300人，高峰时期用工人数超过1000人，除正式员工外，其余均通过劳务派遣方式用工，劳务派遣用工比例存在超过《劳务派遣暂行规定》规定的 10%上限的情形。</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>['详细说明你公司就本次重大资产重组事项的筹划过程', '报送内幕知情人名单', '自查内幕信息知 情人登记及内幕信息管理情况', '核实内幕信息知情人近期股票交易情况']</t>
+          <t>['苏州郎克斯是否存在因上述事项被相应主管部门处罚的风险', '苏州郎克斯降低劳务派遣用工比例的具体措施及其合法合规性，并说明相关措施对苏州郎克斯生产经营及成本费用的影响', '结合报告期内标的公司劳务派遣人数规模、后续被处罚风险、拟采取措施等，披露前述事项对本次交易的影响']</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>关于对四川金时科技股份有限公司的 关注函</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>其他</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>预案披露，截至 2023 年 12 月 31 日，标的公司苏州郎克斯正式员工人数约300人，高峰时期用工人数超过1000人，除正式员工外，其余均通过劳务派遣方式用工，劳务派遣用工比例存在超过《劳务派遣暂行规定》规定的 10%上限的情形。</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>['苏州郎克斯是否存在因上述事项被相应主管部门处罚的风险', '苏州郎克斯降低劳务派遣用工比例的具体措施及其合法合规性，并说明相关措施对苏州郎克斯生产经营及成本费用的影响', '结合报告期内标的公司劳务派遣人数规模、后续被处罚风险、拟采取措施等，披露前述事项对本次交易的影响']</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>公司治理和内部控制问题</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -836,47 +1236,97 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>公告显示， 本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业。请你公司：（1）结合自身以及标的公司财务数据详细说明本次交易构成重大资产重组的测算过程；（2）详细说明你公司进入新业务领域的原因，在标的业务与你公司现有主营业务存在较大差异的情况下，如何实现协同效应；（3）结合你公司进入新领域的专业人员配备、资质情况及业务发展资金储备、资金来源等因素，充分论证进入新业务领域的可行性，收购完成后能否对标的资产实施有效控制；（4）详细说明新领域的行业竞争情况、平均盈利水平，并说明标的公司的主要业务模式、核心竞争力；（5）综合前述情况，详细说明本次重组是否符合《重大资产重组管理办法》第十一条有关有利于增强上市公司核心竞争力、有利于上市公司形成或者保持健全有效的法人治理结构等。</t>
+          <t>其他</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业，需要详细说明你公司进入新业务领域的原因、可行性以及本次重组是否符合《重大资产重组管理办法》的相关规定。</t>
+          <t>因筹划本次发行股份购买资产事项，公司申请2024年1月3日起股票停牌。结合停牌前 6 个月内公司前十大股东变化情况</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>['详细说明本次交易构成重大资产重组的测算过程', '详细说明你公司进入新业务领域的原因', '论证进入新业务领域的可行性', '详细说明新领域的行业竞争情况、平均盈利水平', '说明标的公司的主要业务模式、核心竞争力', '详细说明本次重组是否符合《重大资产重组管理办法》的相关规定']</t>
+          <t>['自查内幕信息知情人登记及内幕信息管理情况，核实公司提交的内幕信息知情人名单是否真实、准确、完整', '补充披露本次重大资产重组的筹划过程，包括但不限于主要时间节点、参与知情人员、商议及决策内容，说明是否存在内幕信息提前泄露情形']</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>关于对四川金时科技股份有限公司的 关注函</t>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>深圳证券交易所</t>
+          <t>上海证券交易所</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>关注函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>四川金时科技股份有限公司</t>
+          <t>哈森商贸 （中国）股份有限公司</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0067</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2024年3月26日</t>
+          <t>二〇二四年一月二十四日</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>其他</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>因筹划本次发行股份购买资产事项，公司申请2024年1月3日起股票停牌。结合停牌前 6 个月内公司前十大股东变化情况</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>['自查内幕信息知情人登记及内幕信息管理情况，核实公司提交的内幕信息知情人名单是否真实、准确、完整', '补充披露本次重大资产重组的筹划过程，包括但不限于主要时间节点、参与知情人员、商议及决策内容，说明是否存在内幕信息提前泄露情形']</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>市场操纵和内幕交易问题</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>关于哈森商贸 （中国）股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的问询函</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>上证公函</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>哈森商贸 （中国）股份有限公司</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>0067</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>二〇二四年一月二十四日</t>
         </is>
       </c>
     </row>
@@ -886,17 +1336,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>你公司2023年度业绩预告显示， 预计 2023年实现营业收入 3,200.00 万元至3,500.00 万元，实现 归属于母公司净利润为亏损4,000.00万元至4,600.00 万元 ，根据本所《股票上市规则》相关规定，你公司股票将可能于 2023年年报披露后被本所实施退市风险警示处理，请严格对照本所相关规则，做好风险提示工作。</t>
+          <t>你公司于 2024年3月22日晚间披露 《 股票交易 异常波动公告》，称公司对有关事项进行了核查，公司不存在应披露而未披露的重大事项，也不存在处于筹划阶段的重大事项， 3月24日晚间你公司就此予以更正。 请你公司 就前述信息披露差错的原因予以自查并说明，包括不限于重大事项的内部信息管理、内部核查机制、信息披露内部审查流程等是否完善，相关流程执行中存在的问题，以及整改情况等。</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>你公司2023年度业绩预告显示，预计亏损较大，根据相关规定，你公司股票将可能面临退市风险警示处理。</t>
+          <t>你公司披露的《 股票交易 异常波动公告》存在信息披露差错，需要进行自查并说明。</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>['严格对照本所相关规则，做好风险提示工作']</t>
+          <t>['自查并说明信息披露差错的原因', '重大事项的内部信息管理情况', '内部核查机制情况', '信息披露内部审查流程情况', '相关流程执行中存在的问题', '整改情况']</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -925,6 +1375,56 @@
         </is>
       </c>
       <c r="J10" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>你公司于 2024年3月22日晚间披露 《 股票交易 异常波动公告》，称公司对有关事项进行了核查，公司不存在应披露而未披露的重大事项，也不存在处于筹划阶段的重大事项， 3月24日晚间你公司就此予以更正。 请你公司 就前述信息披露差错的原因予以自查并说明，包括不限于重大事项的内部信息管理、内部核查机制、信息披露内部审查流程等是否完善，相关流程执行中存在的问题，以及整改情况等。</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>你公司披露的《 股票交易 异常波动公告》存在信息披露差错，需要进行自查并说明。</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>['自查并说明信息披露差错的原因', '重大事项的内部信息管理情况', '内部核查机制情况', '信息披露内部审查流程情况', '相关流程执行中存在的问题', '整改情况']</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>信息披露问题</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
         <is>
           <t>2024年3月26日</t>
         </is>
@@ -936,47 +1436,97 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>关于交易方案</t>
+          <t>本次重组提示性公告披露前， 你公司股价涨幅较大并达到异常波动标准。 请详细说明你公司就本次重大资产重组事项的筹划过程，包括不限于重要时间节点、具体参与人员、筹划事项内容等，并报送内幕知情人名单。请自查内幕信息知 情人登记及内幕信息管理情况，并核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况，说明是否存在内幕信息提前泄露的情形。</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>预案显示，公司拟向贾磊等14名交易对方发行股份并支付现金收购北京领为军融科技有限公司（以下简称标的公司）100%股权。交易对方中，贾磊存在一致行动人邢台领诺、邢台雅惠，合计持有标的公司 41.41%的股权,其他交易对方中包含邢台领擎、科实华盈、力高贰号等多家合伙企业。</t>
+          <t>本次重组提示性公告披露前，你公司股价涨幅较大并达到异常波动标准，可能存在内幕信息提前泄露的情形。</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['（1）除预案披露的一致行动关系外，贾磊与邢台领擎等其他交易对方是否存在关联关系、一致行动关系和其他潜在利益安排；（2）结合预案中 2022 年标的公司初步预计需要确认股份支付费用约 1,200 万元的情况，说明标的公司股份支付费用产生的具体原因，包括但不限于对象、时间、股份支付方式、估值、支付作价、公允价格及确定依据和其他相关安排，并说明本次交易的预计估值区间与前期股份支付对应估值是否存在差异及原因；（3）结合问题（1）和问题（2） ，说明本次向交易对方发行股份是否可能影响上市公司控制权稳定性，本次交易是否将导致上市公司主营业务发生根本变化，是否可能构成《重大资产重组管理办法》规定的重组上市情形。']</t>
+          <t>['详细说明你公司就本次重大资产重组事项的筹划过程', '报送内幕知情人名单', '自查内幕信息知 情人登记及内幕信息管理情况', '核实内幕信息知情人近期股票交易情况']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>上海证券交易所</t>
+          <t>深圳证券交易所</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>上证公函</t>
+          <t>关注函</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>展鹏科技股份有限公司</t>
+          <t>四川金时科技股份有限公司</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3419</t>
+          <t>未知</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>二〇二三年十二月一日</t>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>本次重组提示性公告披露前， 你公司股价涨幅较大并达到异常波动标准。 请详细说明你公司就本次重大资产重组事项的筹划过程，包括不限于重要时间节点、具体参与人员、筹划事项内容等，并报送内幕知情人名单。请自查内幕信息知 情人登记及内幕信息管理情况，并核实控股股东及实控人、公司董事、监事、高级管理人员、 交易对手方及其他相关方等内幕信息知情人近期股票交易情况，说明是否存在内幕信息提前泄露的情形。</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>本次重组提示性公告披露前，你公司股价涨幅较大并达到异常波动标准，可能存在内幕信息提前泄露的情形。</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>['详细说明你公司就本次重大资产重组事项的筹划过程', '报送内幕知情人名单', '自查内幕信息知 情人登记及内幕信息管理情况', '核实内幕信息知情人近期股票交易情况']</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>市场操纵和内幕交易问题</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
         </is>
       </c>
     </row>
@@ -986,47 +1536,97 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>关于交易对方</t>
+          <t>公告显示， 本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业。请你公司：（1）结合自身以及标的公司财务数据详细说明本次交易构成重大资产重组的测算过程；（2）详细说明你公司进入新业务领域的原因，在标的业务与你公司现有主营业务存在较大差异的情况下，如何实现协同效应；（3）结合你公司进入新领域的专业人员配备、资质情况及业务发展资金储备、资金来源等因素，充分论证进入新业务领域的可行性，收购完成后能否对标的资产实施有效控制；（4）详细说明新领域的行业竞争情况、平均盈利水平，并说明标的公司的主要业务模式、核心竞争力；（5）综合前述情况，详细说明本次重组是否符合《重大资产重组管理办法》第十一条有关有利于增强上市公司核心竞争力、有利于上市公司形成或者保持健全有效的法人治理结构等。</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>预案显示：本次发行股份的交易对方为标的公司的 14名股东，其中包括 7家合伙企业。</t>
+          <t>本次重组收购标的青岛展诚注册资本为 489万元，属于软件和信息技术服务业，需要详细说明你公司进入新业务领域的原因、可行性以及本次重组是否符合《重大资产重组管理办法》的相关规定。</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['（1）交易对方穿透后的合计人数，说明是否超过 200 人，是否符合《非上市公众公司监管指引第 4 号》相关规定；（2）交易对方是否专为本次交易设立，如是，补充披露交易完成后最终出资的法人或自然人持有合伙企业份额的锁定安排。']</t>
+          <t>['详细说明本次交易构成重大资产重组的测算过程', '详细说明你公司进入新业务领域的原因', '论证进入新业务领域的可行性', '详细说明新领域的行业竞争情况、平均盈利水平', '说明标的公司的主要业务模式、核心竞争力', '详细说明本次重组是否符合《重大资产重组管理办法》的相关规定']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>上海证券交易所</t>
+          <t>深圳证券交易所</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>上证公函</t>
+          <t>关注函</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>展鹏科技股份有限公司</t>
+          <t>四川金时科技股份有限公司</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3419</t>
+          <t>未知</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>二〇二三年十二月一日</t>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>你公司2023年度业绩预告显示， 预计 2023年实现营业收入 3,200.00 万元至3,500.00 万元，实现 归属于母公司净利润为亏损4,000.00万元至4,600.00 万元 ，根据本所《股票上市规则》相关规定，你公司股票将可能于 2023年年报披露后被本所实施退市风险警示处理，请严格对照本所相关规则，做好风险提示工作。</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>你公司2023年度业绩预告显示，预计亏损较大，根据相关规定，你公司股票将可能面临退市风险警示处理。</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['严格对照本所相关规则，做好风险提示工作']</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>业绩预报问题</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>深圳证券交易所</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>关注函</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>四川金时科技股份有限公司</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>未知</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>2024年3月26日</t>
         </is>
       </c>
     </row>
@@ -1036,49 +1636,71 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>关于标的核心竞争力</t>
+          <t>你公司2023年度业绩预告显示， 预计 2023年实现营业收入 3,200.00 万元至3,500.00 万元，实现 归属于母公司净利润为亏损4,000.00万元至4,600.00 万元 ，根据本所《股票上市规则》相关规定，你公司股票将可能于 2023年年报披露后被本所实施退市风险警示处理，请严格对照本所相关规则，做好风险提示工作。</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>预案显示，标的公司主营业务为军事航空仿真系列产品的研制、生产及相关技术服务，核心产品为“通用数字空战仿真系统”，受专业方向和相关资质许可限制，民营军事仿真市场的准入门槛较高，标的公司形成了多项拥有自主知识产权的现金技术，人才及团队优势也是标的公司核心竞争力之一。</t>
+          <t>你公司2023年度业绩预告显示，预计亏损较大，根据相关规定，你公司股票将可能面临退市风险警示处理。</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['（1）结合标的公司所在行业市场规模、竞争格局、发展趋势、产业政策、资质许可要求、同行业主要竞争对手情况等，进一步说明标的公司的核心竞争力；（2）结合标的公司产品自主知识产权的取得情况，说明标的公司核心产品是否具备足够的技术先进性及技术壁垒，并充分提示技术迭代风险；（3）结合标的公司核心技术人员的学历构成、相关履历、在标的公司的工作年限等，进一步说明标的公司的人才稳定性情况及竞争优势。']</t>
+          <t>['严格对照本所相关规则，做好风险提示工作']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
+          <t>关于对四川金时科技股份有限公司的 关注函</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>上海证券交易所</t>
+          <t>深圳证券交易所</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>上证公函</t>
+          <t>关注函</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>展鹏科技股份有限公司</t>
+          <t>四川金时科技股份有限公司</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3419</t>
+          <t>未知</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>二〇二三年十二月一日</t>
-        </is>
-      </c>
+          <t>2024年3月26日</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>关于交易方案</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>预案显示，公司拟向贾磊等14名交易对方发行股份并支付现金收购北京领为军融科技有限公司（以下简称标的公司）100%股权。交易对方中，贾磊存在一致行动人邢台领诺、邢台雅惠，合计持有标的公司 41.41%的股权,其他交易对方中包含邢台领擎、科实华盈、力高贰号等多家合伙企业。</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>['（1）除预案披露的一致行动关系外，贾磊与邢台领']</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1086,17 +1708,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>关于标的财务状况</t>
+          <t>关于交易方案</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>预案显示，近两年一期标的公司经营业绩波动较大，2022 年营业收入和净利润同比分别增长 81.97%、83.17%，但 2023 年 1-10 月，标的公司实现的营业收入和净利润分别仅达到 2022 年全年的 61.92%和 47.44%。2021 年末，标的公司所有者权益合计为-4,061.85万元。</t>
+          <t>预案显示，公司拟向贾磊等14名交易对方发行股份并支付现金收购北京领为军融科技有限公司（以下简称标的公司）100%股权。交易对方中，贾磊存在一致行动人邢台领诺、邢台雅惠，合计持有标的公司 41.41%的股权,其他交易对方中包含邢台领擎、科实华盈、力高贰号等多家合伙企业。</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['（1）标的公司报告期内经营业绩波动较大的具体原因，相关业绩表现是否与同业公司存在较大差异及其合理性；（2）结合标的公司获取订单的主要方式、在手订单及执行情况、收入确认政策等，是否存在业绩持续下滑风险；（3）标的公司近两年一期前五大客户的销售额及占比、销售模式、是否为关联方，结合主要客户变动情况和客户集中度，说明标的公司是否存在对重大客户依赖的情形及关键客户流失风险；（4）标的公司近两年一期的资产负债的具体构成、资产负债大幅变化的具体原因，收购完成后标的公司相关债务的偿付安排，并结合公司目前的资金状况，说明其是否可能对公司流动性造成不利影响和具体应对措施。']</t>
+          <t>['（1）除预案披露的一致行动关系外，贾磊与邢台领擎等其他交易对方是否存在关联关系、一致行动关系和其他潜在利益安排；（2）结合预案中 2022 年标的公司初步预计需要确认股份支付费用约 1,200 万元的情况，说明标的公司股份支付费用产生的具体原因，包括但不限于对象、时间、股份支付方式、估值、支付作价、公允价格及确定依据和其他相关安排，并说明本次交易的预计估值区间与前期股份支付对应估值是否存在差异及原因；（3）结合问题（1）和问题（2） ，说明本次向交易对方发行股份是否可能影响上市公司控制权稳定性，本次交易是否将导致上市公司主营业务发生根本变化，是否可能构成《重大资产重组管理办法》规定的重组上市情形。']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1129,6 +1751,16 @@
           <t>二〇二三年十二月一日</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1136,17 +1768,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>关于跨界收购</t>
+          <t>关于交易对方</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>预案显示，公司主营电梯门系统等电梯零部件业务。前期公告显示，公司曾于2020年披露跨界重组预案，拟收购主营换电型新能源汽车零部件等业务的伯坦科技， 2021 年 1 月公告终止重组。本次公司拟再次跨界收购，标的公司主营军事航空仿真系列产品等业务，与公司主营业务不具有协同效应。</t>
+          <t>预案显示：本次发行股份的交易对方为标的公司的 14名股东，其中包括 7家合伙企业。</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['（1）多次筹划收购与公司主营业务不具有协同效应标的公司的具体原因，充分论证收购的必要性，交易是否符合《重大资产重组管理办法》第十一条的有关规定；（2）结合公司现阶段主营业务、人才储备等情况是否具备足够的整合管控标的公司的能力，审慎推进本次收购事项，并严格按照规则要求履行信息披露义务。']</t>
+          <t>['（1）交易对方穿透后的合计人数，说明是否超过 200 人，是否符合《非上市公众公司监管指引第 4 号》相关规定；（2）交易对方是否专为本次交易设立，如是，补充披露交易完成后最终出资的法人或自然人持有合伙企业份额的锁定安排。']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1179,6 +1811,16 @@
           <t>二〇二三年十二月一日</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1186,17 +1828,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>关于内幕信息</t>
+          <t>关于标的核心竞争力</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>因筹划重大资产重组，公司于 2023 年11 月 6 日起停牌。公司提交停牌申请当日，停牌前筹划本次重大资产重组事项的具体协商、参与知情人自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。</t>
+          <t>预案显示，标的公司主营业务为军事航空仿真系列产品的研制、生产及相关技术服务，核心产品为“通用数字空战仿真系统”，受专业方向和相关资质许可限制，民营军事仿真市场的准入门槛较高，标的公司形成了多项拥有自主知识产权的现金技术，人才及团队优势也是标的公司核心竞争力之一。</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['（1）停牌前筹划本次重大资产重组事项的具体协商、参与知情人；（2）自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。']</t>
+          <t>['（1）结合标的公司所在行业市场规模、竞争格局、发展趋势、产业政策、资质许可要求、同行业主要竞争对手情况等，进一步说明标的公司的核心竞争力；（2）结合标的公司产品自主知识产权的取得情况，说明标的公司核心产品是否具备足够的技术先进性及技术壁垒，并充分提示技术迭代风险；（3）结合标的公司核心技术人员的学历构成、相关履历、在标的公司的工作年限等，进一步说明标的公司的人才稳定性情况及竞争优势。']</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1229,6 +1871,16 @@
           <t>二〇二三年十二月一日</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1236,22 +1888,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>关于交易标的的并表</t>
+          <t>关于标的财务状况</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>预案显示，交易完成后，上市公司、上海宝信软件股份有限公司（以下简称“宝信软件”）分别持有上海地铁电子科技有限公司（以下简称“地铁电科”）50%股权，股权比例相同；上市公司、上海地铁维护保障有限公司（以下简称 “维保公司 ”）将分别持有上海地铁物业管理有限公司（以下简称 “地铁物业 ”）51%、49%股权，股权比例相近。</t>
+          <t>预案显示，近两年一期标的公司经营业绩波动较大，2022 年营业收入和净利润同比分别增长 81.97%、83.17%，但 2023 年 1-10 月，标的公司实现的营业收入和净利润分别仅达到 2022 年全年的 61.92%和 47.44%。2021 年末，标的公司所有者权益合计为-4,061.85万元。</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['结合地铁电科、地铁物业的公司章程规定、董事会席位安排、经营决策具体安排及重大事项表决安排等，说明交易后上市公司能否对交易标的实施控制、能否将其纳入合并报表及相应会计处理的合理性。']</t>
+          <t>['（1）标的公司报告期内经营业绩波动较大的具体原因，相关业绩表现是否与同业公司存在较大差异及其合理性；（2）结合标的公司获取订单的主要方式、在手订单及执行情况、收入确认政策等，是否存在业绩持续下滑风险；（3）标的公司近两年一期前五大客户的销售额及占比、销售模式、是否为关联方，结合主要客户变动情况和客户集中度，说明标的公司是否存在对重大客户依赖的情形及关键客户流失风险；（4）标的公司近两年一期的资产负债的具体构成、资产负债大幅变化的具体原因，收购完成后标的公司相关债务的偿付安排，并结合公司目前的资金状况，说明其是否可能对公司流动性造成不利影响和具体应对措施。']</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1266,19 +1918,29 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>上海申通地铁股份有限公司</t>
+          <t>展鹏科技股份有限公司</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3403</t>
+          <t>3419</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>二〇二三年十一月二十七日</t>
-        </is>
-      </c>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1286,22 +1948,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>关于独立性</t>
+          <t>关于跨界收购</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>预案显示，地铁电科主营轨道交通车辆及相关系统部件的维护、维修，地铁物业主营列车等保洁、车站服务设施综合管理。</t>
+          <t>预案显示，公司主营电梯门系统等电梯零部件业务。前期公告显示，公司曾于2020年披露跨界重组预案，拟收购主营换电型新能源汽车零部件等业务的伯坦科技， 2021 年 1 月公告终止重组。本次公司拟再次跨界收购，标的公司主营军事航空仿真系列产品等业务，与公司主营业务不具有协同效应。</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['补充披露： （1）地铁电科、地铁物业报告期内是否存在关联销售，若存在，请披露报告期内金额、占比、定价模式及定价公允性；（2）本次交易前后关联交易的金额及规模占比变化情况，本次交易是否有利于减少关联交易、增强上市公司独立性；（3）上市公司后续保持关联交易定价公允、减少和规范关联交易的具体措施。']</t>
+          <t>['（1）多次筹划收购与公司主营业务不具有协同效应标的公司的具体原因，充分论证收购的必要性，交易是否符合《重大资产重组管理办法》第十一条的有关规定；（2）结合公司现阶段主营业务、人才储备等情况是否具备足够的整合管控标的公司的能力，审慎推进本次收购事项，并严格按照规则要求履行信息披露义务。']</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1316,19 +1978,29 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>上海申通地铁股份有限公司</t>
+          <t>展鹏科技股份有限公司</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3403</t>
+          <t>3419</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>二〇二三年十一月二十七日</t>
-        </is>
-      </c>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1336,22 +2008,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>关于地铁电科资产负债率</t>
+          <t>关于内幕信息</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>地铁电科报告期内资产负债率分别为74%、70%和69%，远高于上市公司2023年三季度末资产负债率39.53%。</t>
+          <t>因筹划重大资产重组，公司于 2023 年11 月 6 日起停牌。公司提交停牌申请当日，停牌前筹划本次重大资产重组事项的具体协商、参与知情人自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['补充披露： （1）报告期内地铁电科的资产、负债主要构成，结合自身经营情况、融资来源及融资结构等，说明地铁电科资产负债率较高的原因及合理性；（2）说明此次交易是否会对上市公司财务结构产生重大影响，交易完成后上市公司资产负债率是否处于合理水平。']</t>
+          <t>['（1）停牌前筹划本次重大资产重组事项的具体协商、参与知情人；（2）自查内幕信息知情人登记及内幕信息管理情况、申请停牌当日市场传闻的具体来源、相关内幕信息知情人是否涉嫌内幕交易等违法违规情形，并核实向我部报送的内幕信息知情人名单的真实、准确和完整性。']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
+          <t>关于对展鹏科技股份有限公司发行股份及支付现金购买资产并募集配套资金暨关联交易预案的监管问询函</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1366,19 +2038,29 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>上海申通地铁股份有限公司</t>
+          <t>展鹏科技股份有限公司</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>3403</t>
+          <t>3419</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>二〇二三年十一月二十七日</t>
-        </is>
-      </c>
+          <t>二〇二三年十二月一日</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1386,17 +2068,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>关于地铁电科业绩</t>
+          <t>关于交易标的的并表</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>预案显示，地铁电科报告期内实现营业收入分别为17,696.24万元、13,632.78万元及9,728.3万元，净利润分别为 2,357.88 万元、1,389.45 万元、604.54 万元，净利率分别为13%、10%、6%，净利率持续下降；经营活动产生的现金流量净额分别为-515.36万元、-1,522.17万元及774万元，波动较大。</t>
+          <t>预案显示，交易完成后，上市公司、上海宝信软件股份有限公司（以下简称“宝信软件”）分别持有上海地铁电子科技有限公司（以下简称“地铁电科”）50%股权，股权比例相同；上市公司、上海地铁维护保障有限公司（以下简称 “维保公司 ”）将分别持有上海地铁物业管理有限公司（以下简称 “地铁物业 ”）51%、49%股权，股权比例相近。</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['补充披露： （1）结合地铁电科业务开展情况，包括主要客户变化、销售模式、收入确认方式等，说明公司营业收入、净利率下降的原因及合理性；（2）结合公司对客户及供应商的结算方式，说明经营活动现金流量净额波动较大的原因及合理性。']</t>
+          <t>['结合地铁电科、地铁物业的公司章程规定、董事会席位安排、经营决策具体安排及重大事项表决安排等，说明交易后上市公司能否对交易标的实施控制、能否将其纳入合并报表及相应会计处理的合理性。']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1429,6 +2111,16 @@
           <t>二〇二三年十一月二十七日</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1436,17 +2128,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>关于地铁物业业绩</t>
+          <t>关于独立性</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>预案显示，地铁物业处于劳动密集型行业，2022 年实现营业收入 21,096.63 万元，同比增长 21%；净利润为 401.34 万元，同比下降 53%，经营活动现金净额为-2,074.36 万元，2021 年同期为-382.58 万元，净利润、经营活动现金净额的变动趋势与营业收入相反，且 2022 年净利率仅为 2%。</t>
+          <t>预案显示，地铁电科主营轨道交通车辆及相关系统部件的维护、维修，地铁物业主营列车等保洁、车站服务设施综合管理。</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['补充披露： （1）地铁物业的盈利模式，净利率较低的原因及合理性，是否与同行业可比公司相一致；（2）结合前述问题分析、地铁物业经营情况、收入确认方式与期间费用变化等，说明2022年收入大幅提升，但净利润大幅下滑的原因及合理性；（3）结合主要客户及供应商变化情况、结算政策等，说明经营活动现金净额与收入变化不匹配的原因及合理性。']</t>
+          <t>['补充披露： （1）地铁电科、地铁物业报告期内是否存在关联销售，若存在，请披露报告期内金额、占比、定价模式及定价公允性；（2）本次交易前后关联交易的金额及规模占比变化情况，本次交易是否有利于减少关联交易、增强上市公司独立性；（3）上市公司后续保持关联交易定价公允、减少和规范关联交易的具体措施。']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1479,6 +2171,16 @@
           <t>二〇二三年十一月二十七日</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1486,17 +2188,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>关于地铁电科核心竞争力</t>
+          <t>关于地铁电科资产负债率</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>预案显示，地铁电科属于技术密集型行业，核心管理人员及技术人员对其发展至关重要。</t>
+          <t>地铁电科报告期内资产负债率分别为74%、70%和69%，远高于上市公司2023年三季度末资产负债率39.53%。</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['结合地铁电科所处细分行业竞争格局、同行业竞争对手情况、现有技术储备、人员配置等，说明地铁电科核心竞争力，及此次交易完成后，公司拟采取何种措施整合地铁电科的技术和相关人员。']</t>
+          <t>['补充披露： （1）报告期内地铁电科的资产、负债主要构成，结合自身经营情况、融资来源及融资结构等，说明地铁电科资产负债率较高的原因及合理性；（2）说明此次交易是否会对上市公司财务结构产生重大影响，交易完成后上市公司资产负债率是否处于合理水平。']</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1529,6 +2231,16 @@
           <t>二〇二三年十一月二十七日</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1536,22 +2248,22 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>关于本次交易情况</t>
+          <t>关于地铁电科业绩</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>你公司披露《关于使用超募资金对外投资的公告》称，公司拟使用超募资金（含利息收入、理财收益等）9,023.81万元用于收购福昕鲲鹏（北京）信息科技有限公司（以下简称福昕鲲鹏或标的公司）38.27%的股权，本次股权收购完成后，你公司将持有标的公司73.24%的股权，取得对标的公司的控制权。</t>
+          <t>预案显示，地铁电科报告期内实现营业收入分别为17,696.24万元、13,632.78万元及9,728.3万元，净利润分别为 2,357.88 万元、1,389.45 万元、604.54 万元，净利率分别为13%、10%、6%，净利率持续下降；经营活动产生的现金流量净额分别为-515.36万元、-1,522.17万元及774万元，波动较大。</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['结合标的公司的实际经营情况、研发团队、研发成果、技术实力、行业地位、近一年同行业公司的并购估值情况等，说明标的公司股东权益评估价值与公司净资产差异较大的原因、依据及其合理性；', '本次交易约定的三期付款先决条件，并说明公司本次交易支付安排是否符合商业惯例、是否有利于保障公司及中小投资者利益；', '公司实施此次股权收购的必要性、决策过程，未设置业绩补偿安排的原因，以及拟采取何种措施保证投资收益、保障公司及中小投资者利益。']</t>
+          <t>['补充披露： （1）结合地铁电科业务开展情况，包括主要客户变化、销售模式、收入确认方式等，说明公司营业收入、净利率下降的原因及合理性；（2）结合公司对客户及供应商的结算方式，说明经营活动现金流量净额波动较大的原因及合理性。']</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1561,24 +2273,34 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>上证科创公函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司</t>
+          <t>上海申通地铁股份有限公司</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>0034</t>
+          <t>3403</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>二〇二四年三月二十五日</t>
-        </is>
-      </c>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1586,22 +2308,22 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>关于标的公司经营情况</t>
+          <t>关于地铁物业业绩</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>公告显示，标的公司净资产为负，最近一年及一期净利润持续亏损，2023年1-10月净亏损达到7,471.04万元。</t>
+          <t>预案显示，地铁物业处于劳动密集型行业，2022 年实现营业收入 21,096.63 万元，同比增长 21%；净利润为 401.34 万元，同比下降 53%，经营活动现金净额为-2,074.36 万元，2021 年同期为-382.58 万元，净利润、经营活动现金净额的变动趋势与营业收入相反，且 2022 年净利率仅为 2%。</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['标的公司的资产负债结构、主要资产构成，标的公司的资产是否足以支持业务运营；', '标的公司财产抵押及贷款的现状，说明标的公司是否存在债务清偿风险；', '标的公司最近三年的主要财务数据及业务发展情况，并说明标的公司最近一年及一期连续亏损的原因以及本次收购是否有利于提高上市公司盈利能力。']</t>
+          <t>['补充披露： （1）地铁物业的盈利模式，净利率较低的原因及合理性，是否与同行业可比公司相一致；（2）结合前述问题分析、地铁物业经营情况、收入确认方式与期间费用变化等，说明2022年收入大幅提升，但净利润大幅下滑的原因及合理性；（3）结合主要客户及供应商变化情况、结算政策等，说明经营活动现金净额与收入变化不匹配的原因及合理性。']</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1611,24 +2333,34 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>上证科创公函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司</t>
+          <t>上海申通地铁股份有限公司</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>0034</t>
+          <t>3403</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>二〇二四年三月二十五日</t>
-        </is>
-      </c>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1636,22 +2368,22 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>关于后续整合安排</t>
+          <t>关于地铁电科核心竞争力</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>公告显示，本次交易完成后，公司将持有标的公司73.24%的股权，取得对标的公司的控制权，标的公司将纳入公司合并报表范围。</t>
+          <t>预案显示，地铁电科属于技术密集型行业，核心管理人员及技术人员对其发展至关重要。</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['本次交易后的董事会及管理层的人员安排，以及你公司在业务、资产、财务、人员等方面拟采取的其他整合管控措施，并说明相关安排或措施如何保障对标的公司实现有效整合；', '收购后对标的公司有无进一步资金投入规划，有无收购相关业务领域其他资产的计划，如有，请披露预计投入金额及具体内容；', '结合标的公司产品的具体种类、主要客户及在手订单，细分市场总体规模及行业竞争状况等因素预计标的公司未来三年的收入流情况，是否能够实现业绩扭亏为盈，并说明改善标的公司经营情况的具体举措。']</t>
+          <t>['结合地铁电科所处细分行业竞争格局、同行业竞争对手情况、现有技术储备、人员配置等，说明地铁电科核心竞争力，及此次交易完成后，公司拟采取何种措施整合地铁电科的技术和相关人员。']</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+          <t>关于对上海申通地铁股份有限公司重大资产购买暨关联交易预案的问询函</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1661,24 +2393,34 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>上证科创公函</t>
+          <t>上证公函</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>福建福昕软件开发股份有限公司</t>
+          <t>上海申通地铁股份有限公司</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>0034</t>
+          <t>3403</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>二〇二四年三月二十五日</t>
-        </is>
-      </c>
+          <t>二〇二三年十一月二十七日</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1686,22 +2428,22 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>公司2023年度业绩情况</t>
+          <t>关于本次交易情况</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>公司2023年财务数据对公司具有较大影响，根据本所《股票上市规则》第 13.1.1条等有关规定，现请你公司进一步核实并补充披露以下事项。</t>
+          <t>你公司披露《关于使用超募资金对外投资的公告》称，公司拟使用超募资金（含利息收入、理财收益等）9,023.81万元用于收购福昕鲲鹏（北京）信息科技有限公司（以下简称福昕鲲鹏或标的公司）38.27%的股权，本次股权收购完成后，你公司将持有标的公司73.24%的股权，取得对标的公司的控制权。</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['区分产品类别披露主营业务的开展情况，包括开展期限、采购及销售模式、收入确认方式等，说明是否为贸易业务', '各业务板块的主要供应商和客户名称、所涉关联关系、业务内容及报告期内变化情况，结合主要合同条款及公司承担的责任和义务等情况，说明报告期内业务收入确认的依据及政策，是否符合《企业会计准则》的规定，是否存在提前确认收入的情形', '结合经营情况、财务状况及变化趋势，说明持续经营能力是否存在重大不确定性，并充分提示风险']</t>
+          <t>['结合标的公司的实际经营情况、研发团队、研发成果、技术实力、行业地位、近一年同行业公司的并购估值情况等，说明标的公司股东权益评估价值与公司净资产差异较大的原因、依据及其合理性；', '本次交易约定的三期付款先决条件，并说明公司本次交易支付安排是否符合商业惯例、是否有利于保障公司及中小投资者利益；', '公司实施此次股权收购的必要性、决策过程，未设置业绩补偿安排的原因，以及拟采取何种措施保证投资收益、保障公司及中小投资者利益。']</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>关于精伦电子股份有限公司业绩预告相关事项的问询函</t>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1711,24 +2453,34 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>问询函</t>
+          <t>上证科创公函</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>精伦电子股份有限公司</t>
+          <t>福建福昕软件开发股份有限公司</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0034</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>二〇二四年一月二十六日</t>
-        </is>
-      </c>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1736,22 +2488,22 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>营业收入扣除项目及其具体情况</t>
+          <t>关于标的公司经营情况</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>请公司补充披露营业收入扣除项目及其具体情况 ，并逐条对照《上海证券交易所上市公司自律监管指南第 2号—业务办理》附件第七号《财务类退市指标：营业收入扣除》有关规定，说明公司未扣除收入的相关业务是否存在应扣除收入未按规定扣除的情况。如扣除后的营业收入等财务指标触及财务类退市情形的，公司股票将被实施退市风险警示 ，请公司充分提示相关风险。</t>
+          <t>公告显示，标的公司净资产为负，最近一年及一期净利润持续亏损，2023年1-10月净亏损达到7,471.04万元。</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['营业收入扣除项目及其具体情况']</t>
+          <t>['标的公司的资产负债结构、主要资产构成，标的公司的资产是否足以支持业务运营；', '标的公司财产抵押及贷款的现状，说明标的公司是否存在债务清偿风险；', '标的公司最近三年的主要财务数据及业务发展情况，并说明标的公司最近一年及一期连续亏损的原因以及本次收购是否有利于提高上市公司盈利能力。']</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>关于精伦电子股份有限公司业绩预告相关事项的问询函</t>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1761,24 +2513,34 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>问询函</t>
+          <t>上证科创公函</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>精伦电子股份有限公司</t>
+          <t>福建福昕软件开发股份有限公司</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>未知</t>
+          <t>0034</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>二〇二四年一月二十六日</t>
-        </is>
-      </c>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1786,49 +2548,119 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>关于后续整合安排</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>公告显示，本次交易完成后，公司将持有标的公司73.24%的股权，取得对标的公司的控制权，标的公司将纳入公司合并报表范围。</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['本次交易后的董事会及管理层的人员安排，以及你公司在业务、资产、财务、人员等方面拟采取的其他整合管控措施，并说明相关安排或措施如何保障对标的公司实现有效整合；', '收购后对标的公司有无进一步资金投入规划，有无收购相关业务领域其他资产的计划，如有，请披露预计投入金额及具体内容；', '结合标的公司产品的具体种类、主要客户及在手订单，细分市场总体规模及行业竞争状况等因素预计标的公司未来三年的收入流情况，是否能够实现业绩扭亏为盈，并说明改善标的公司经营情况的具体举措。']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>关于福建福昕软件开发股份有限公司使用超募资金对外投资事项的问询函</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>上证科创公函</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>福建福昕软件开发股份有限公司</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>0034</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>二〇二四年三月二十五日</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>关于江苏迈信林航空科技股份有限公司签订战略框架协议暨开展新业务相关事项的问询</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>江苏迈信林航空科技股份有限公司披露《关于自愿披露签订战略框架协议暨开展新业务的公告》称，公司通过子公司苏州瑞盈智算科技有限公司开展算力服务业务，并与苏州算力科技有限公司签订战略合作框架协议，拟在算力领域开展深度合作，建立长期的战略合作关系。经事后审核，根据《上海证券交易所科创板股票上市规则》第14.1.1条，请你公司就如下信息予以说明并补充披露。</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>['瑞盈智算的股权结构，预计注册资本实缴到位时间', '结合从事算力服务业务所需要的技术、资质、人员条件及市场竞争情况等，说明公司是否具备相关储备，是否具备开展算力服务业务的条件，是否具备竞争优势，并针对性提示风险', '后续服务器采购计划和具体安排，交付是否存在不确定性', '结合公司的自有资金情况，说明相关投资是否影响公司现金流，是否可能导致公司后续存在资金周转风险', '瑞盈智算后续获取银行信贷，是否需要公司提供担保或承担连带责任，结合后续算力服务业务的不确定性，评估可能给公司带来风险并进行针对性风险提示', '截至目前，上市公司已采购60余台服务器，待瑞盈智算正式运营，公司将以公允价格全部划转至瑞盈智算。请公司补充披露相关采购事项是否达到信息披露标准，智算受让公司已采购服务器的具体安排，包括但不限于转让时间、数量、价格等', '苏州算力科技协助瑞盈智算运营管理的具体工作内容及收费模式，苏州算力科技是否具备资金、技术、客户资源等合作条件']</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>江苏迈信林航空科技股份有限公司披露《关于自愿披露签订战略框架协议暨开展新业务的公告》称，公司通过子公司苏州瑞盈智算科技有限公司开展算力服务业务，并与苏州算力科技有限公司签订战略合作框架协议，拟在算力领域开展深度合作，建立长期的战略合作关系。</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['瑞盈智算的股权结构，预计注册资本实缴到位时间', '结合从事算力服务业务所需要的技术、资质、人员条件及市场竞争情况等，说明公司是否具备相关储备，是否具备开展算力服务业务的条件，是否具备竞争优势，并针对性提示风险', '后续服务器采购计划和具体安排，交付是否存在不确定性', '结合公司的自有资金情况，说明相关投资是否影响公司现金流，是否可能导致公司后续存在资金周转风险', '瑞盈智算后续获取银行信贷，是否需要公司提供担保或承担连带责任，结合后续算力服务业务的不确定性，评估可能给公司带来风险并进行针对性风险提示', '相关采购事项是否达到信息披露标准', '智算受让公司已采购服务器的具体安排，包括但不限于转让时间、数量、价格等', '苏州算力科技协助瑞盈智算运营管理的具体工作内容及收费模式，苏州算力科技是否具备资金、技术、客户资源等合作条件']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>关于江苏迈信林航空科技股份有限公司签订战略框架协议暨开展新业务相关事项的问询</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>上海证券交易所</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>上海证券交易所</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>科创公函</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>江苏迈信林航空科技股份有限公司</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>0033</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>2024年3月23日</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>